<commit_message>
add testing notebooks for jump effects, Arrhenius barriers, and plotting individual paths
</commit_message>
<xml_diff>
--- a/P_vs_T_results.xlsx
+++ b/P_vs_T_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nate_schwindt/Projects/eyring_model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B727DC05-18B2-D246-909B-E88DC0AF66B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECDB23BA-2D30-A849-9405-626006581123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="17420" windowHeight="21900" xr2:uid="{F8B1EA0F-A308-4B23-AF40-5EC820F734E9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="7">
   <si>
     <t>T (K)</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>B (m/sec)</t>
+  </si>
+  <si>
+    <t>ave B (m/sec)</t>
   </si>
 </sst>
 </file>
@@ -156,13 +159,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,11 +493,12 @@
   <dimension ref="A1:AS67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+      <selection activeCell="D44" sqref="D44:D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.6640625" customWidth="1"/>
     <col min="15" max="15" width="13.1640625" customWidth="1"/>
@@ -517,6 +521,9 @@
       <c r="C1" t="s">
         <v>3</v>
       </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A2">
@@ -528,6 +535,10 @@
       <c r="C2" t="s">
         <v>1</v>
       </c>
+      <c r="D2">
+        <f>AVERAGE(B2,B8,B14)</f>
+        <v>2.1480346994554405E-5</v>
+      </c>
     </row>
     <row r="3" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -539,6 +550,10 @@
       <c r="C3" t="s">
         <v>1</v>
       </c>
+      <c r="D3">
+        <f>AVERAGE(B3,B9,B15)</f>
+        <v>2.5604753245916383E-5</v>
+      </c>
     </row>
     <row r="4" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -550,6 +565,10 @@
       <c r="C4" t="s">
         <v>1</v>
       </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D55" si="0">AVERAGE(B4,B10,B16)</f>
+        <v>2.9421918155453795E-5</v>
+      </c>
     </row>
     <row r="5" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -560,6 +579,10 @@
       </c>
       <c r="C5" t="s">
         <v>1</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>3.3983109393682904E-5</v>
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
@@ -590,6 +613,10 @@
       <c r="C6" t="s">
         <v>1</v>
       </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>3.8257119245092766E-5</v>
+      </c>
       <c r="W6" s="8"/>
     </row>
     <row r="7" spans="1:45" x14ac:dyDescent="0.2">
@@ -601,6 +628,10 @@
       </c>
       <c r="C7" t="s">
         <v>1</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>4.3086885862082806E-5</v>
       </c>
       <c r="R7" s="4"/>
       <c r="T7" s="4"/>
@@ -727,12 +758,12 @@
       <c r="AE15" s="5"/>
       <c r="AF15" s="9"/>
       <c r="AG15" s="5"/>
-      <c r="AN15" s="12"/>
-      <c r="AO15" s="12"/>
-      <c r="AP15" s="13"/>
-      <c r="AQ15" s="13"/>
-      <c r="AR15" s="12"/>
-      <c r="AS15" s="12"/>
+      <c r="AN15" s="13"/>
+      <c r="AO15" s="13"/>
+      <c r="AP15" s="14"/>
+      <c r="AQ15" s="14"/>
+      <c r="AR15" s="13"/>
+      <c r="AS15" s="13"/>
     </row>
     <row r="16" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A16">
@@ -787,6 +818,10 @@
       </c>
       <c r="C20" t="s">
         <v>2</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>1.0039884606980105E-5</v>
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
@@ -818,6 +853,10 @@
       <c r="C21" t="s">
         <v>2</v>
       </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>1.2126033402422545E-5</v>
+      </c>
       <c r="W21" s="8"/>
     </row>
     <row r="22" spans="1:45" x14ac:dyDescent="0.2">
@@ -830,6 +869,10 @@
       <c r="C22" t="s">
         <v>2</v>
       </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>1.4294667713161648E-5</v>
+      </c>
       <c r="R22" s="4"/>
       <c r="T22" s="4"/>
       <c r="V22" s="4"/>
@@ -844,6 +887,10 @@
       <c r="C23" t="s">
         <v>2</v>
       </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>1.6582457181873137E-5</v>
+      </c>
       <c r="R23" s="4"/>
       <c r="T23" s="4"/>
       <c r="V23" s="4"/>
@@ -858,6 +905,10 @@
       <c r="C24" t="s">
         <v>2</v>
       </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>1.9043586720050759E-5</v>
+      </c>
       <c r="R24" s="4"/>
       <c r="T24" s="4"/>
       <c r="V24" s="4"/>
@@ -871,6 +922,10 @@
       </c>
       <c r="C25" t="s">
         <v>2</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>2.2426483117942158E-5</v>
       </c>
       <c r="R25" s="4"/>
       <c r="T25" s="4"/>
@@ -948,12 +1003,12 @@
       <c r="AE30" s="5"/>
       <c r="AF30" s="9"/>
       <c r="AG30" s="5"/>
-      <c r="AN30" s="12"/>
-      <c r="AO30" s="12"/>
-      <c r="AP30" s="13"/>
-      <c r="AQ30" s="13"/>
-      <c r="AR30" s="12"/>
-      <c r="AS30" s="12"/>
+      <c r="AN30" s="13"/>
+      <c r="AO30" s="13"/>
+      <c r="AP30" s="14"/>
+      <c r="AQ30" s="14"/>
+      <c r="AR30" s="13"/>
+      <c r="AS30" s="13"/>
     </row>
     <row r="31" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A31">
@@ -1085,11 +1140,15 @@
       <c r="A38">
         <v>284.7</v>
       </c>
-      <c r="B38" s="14">
+      <c r="B38" s="12">
         <v>2.2666999999999998E-6</v>
       </c>
       <c r="C38" t="s">
         <v>4</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="0"/>
+        <v>3.3325926181357415E-6</v>
       </c>
       <c r="I38" s="4"/>
       <c r="L38" s="4"/>
@@ -1100,11 +1159,15 @@
       <c r="A39">
         <v>290</v>
       </c>
-      <c r="B39" s="14">
+      <c r="B39" s="12">
         <v>2.8245199999999999E-6</v>
       </c>
       <c r="C39" t="s">
         <v>4</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="0"/>
+        <v>4.0455100594606638E-6</v>
       </c>
       <c r="I39" s="4"/>
       <c r="L39" s="4"/>
@@ -1115,11 +1178,15 @@
       <c r="A40">
         <v>295.8</v>
       </c>
-      <c r="B40" s="14">
+      <c r="B40" s="12">
         <v>3.7446900000000001E-6</v>
       </c>
       <c r="C40" t="s">
         <v>4</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="0"/>
+        <v>5.1825923536012713E-6</v>
       </c>
       <c r="I40" s="4"/>
       <c r="L40" s="4"/>
@@ -1132,11 +1199,15 @@
       <c r="A41">
         <v>301.7</v>
       </c>
-      <c r="B41" s="14">
+      <c r="B41" s="12">
         <v>4.3755200000000004E-6</v>
       </c>
       <c r="C41" t="s">
         <v>4</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="0"/>
+        <v>6.0339553156590187E-6</v>
       </c>
       <c r="J41" s="8"/>
       <c r="T41" s="8"/>
@@ -1145,22 +1216,30 @@
       <c r="A42">
         <v>308.35000000000002</v>
       </c>
-      <c r="B42" s="14">
+      <c r="B42" s="12">
         <v>5.3009700000000002E-6</v>
       </c>
       <c r="C42" t="s">
         <v>4</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="0"/>
+        <v>6.9130251286712408E-6</v>
       </c>
     </row>
     <row r="43" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>313.45</v>
       </c>
-      <c r="B43" s="14">
+      <c r="B43" s="12">
         <v>6.0754100000000002E-6</v>
       </c>
       <c r="C43" t="s">
         <v>4</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="0"/>
+        <v>7.2893870913019731E-6</v>
       </c>
       <c r="W43" s="5"/>
       <c r="X43" s="9"/>
@@ -1171,12 +1250,12 @@
       <c r="AC43" s="5"/>
       <c r="AD43" s="9"/>
       <c r="AE43" s="5"/>
-      <c r="AN43" s="12"/>
-      <c r="AO43" s="12"/>
-      <c r="AP43" s="13"/>
-      <c r="AQ43" s="13"/>
-      <c r="AR43" s="12"/>
-      <c r="AS43" s="12"/>
+      <c r="AN43" s="13"/>
+      <c r="AO43" s="13"/>
+      <c r="AP43" s="14"/>
+      <c r="AQ43" s="14"/>
+      <c r="AR43" s="13"/>
+      <c r="AS43" s="13"/>
     </row>
     <row r="44" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A44">
@@ -1248,7 +1327,7 @@
       <c r="A50">
         <v>284.7</v>
       </c>
-      <c r="B50" s="14">
+      <c r="B50" s="12">
         <v>4.8799999999999999E-6</v>
       </c>
       <c r="C50" t="s">
@@ -1259,7 +1338,7 @@
       <c r="A51">
         <v>290</v>
       </c>
-      <c r="B51" s="14">
+      <c r="B51" s="12">
         <v>5.9800000000000003E-6</v>
       </c>
       <c r="C51" t="s">
@@ -1270,7 +1349,7 @@
       <c r="A52">
         <v>295.8</v>
       </c>
-      <c r="B52" s="14">
+      <c r="B52" s="12">
         <v>7.5800000000000003E-6</v>
       </c>
       <c r="C52" t="s">
@@ -1281,7 +1360,7 @@
       <c r="A53">
         <v>301.7</v>
       </c>
-      <c r="B53" s="14">
+      <c r="B53" s="12">
         <v>8.7499999999999992E-6</v>
       </c>
       <c r="C53" t="s">
@@ -1292,7 +1371,7 @@
       <c r="A54">
         <v>308.35000000000002</v>
       </c>
-      <c r="B54" s="14">
+      <c r="B54" s="12">
         <v>9.8200000000000008E-6</v>
       </c>
       <c r="C54" t="s">
@@ -1303,7 +1382,7 @@
       <c r="A55">
         <v>313.45</v>
       </c>
-      <c r="B55" s="14">
+      <c r="B55" s="12">
         <v>1.01E-5</v>
       </c>
       <c r="C55" t="s">

</xml_diff>